<commit_message>
modified the TopUp.cs file to handle better top up by checking existing card balance.
</commit_message>
<xml_diff>
--- a/final/FinalProject/StudentCredit.xlsx
+++ b/final/FinalProject/StudentCredit.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>StudentID</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>Wells Fargo inc</t>
+  </si>
+  <si>
+    <t>Absa Bank</t>
+  </si>
+  <si>
+    <t>95019925</t>
   </si>
 </sst>
 </file>
@@ -356,7 +362,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D353"/>
+  <dimension ref="A1:F353"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D171" sqref="D171"/>
@@ -426,10 +432,38 @@
       </c>
     </row>
     <row r="5">
-      <c r="D5" s="1"/>
+      <c r="A5" s="0">
+        <v>20115817</v>
+      </c>
+      <c r="B5" s="0">
+        <v>1000</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1">
+        <v>10082900142</v>
+      </c>
     </row>
     <row r="6">
-      <c r="D6" s="1"/>
+      <c r="A6" s="0">
+        <v>0</v>
+      </c>
+      <c r="B6" s="0">
+        <v>100</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1">
+        <v>90030021345</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="0">
+        <v>100</v>
+      </c>
     </row>
     <row r="7">
       <c r="D7" s="1"/>

</xml_diff>